<commit_message>
Updated based on UAT_2023041212
</commit_message>
<xml_diff>
--- a/Test Data/Ajman SuperApp - Test Data.xlsx
+++ b/Test Data/Ajman SuperApp - Test Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="2" windowHeight="7950" windowWidth="20055" xWindow="240" yWindow="60"/>
+    <workbookView activeTab="13" firstSheet="10" windowHeight="7950" windowWidth="20055" xWindow="240" yWindow="60"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" r:id="rId1" sheetId="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="133">
   <si>
     <t>biller</t>
   </si>
@@ -308,9 +308,6 @@
 Reference ID</t>
   </si>
   <si>
-    <t>Email Address Not Updated. Please Try Again</t>
-  </si>
-  <si>
     <t>Biller ADDC Saved Successfully with consumer number 8235355929</t>
   </si>
   <si>
@@ -327,6 +324,115 @@
 4285720304320212
 Reference ID
 FT23093PR6XD</t>
+  </si>
+  <si>
+    <t>DonationName</t>
+  </si>
+  <si>
+    <t>Humaid Bin Rashid AL Nouimi</t>
+  </si>
+  <si>
+    <t>Zakat Fund-Zakat Al Mal</t>
+  </si>
+  <si>
+    <t>Zakat Fund-Al Sadaqat</t>
+  </si>
+  <si>
+    <t>Zakat Fund-Zakat Al Fitr</t>
+  </si>
+  <si>
+    <t>Salik</t>
+  </si>
+  <si>
+    <t>SALIK</t>
+  </si>
+  <si>
+    <t>100.00
+AED
+Donated to
+Humaid Bin Rashid AL Nouimi
+Charity Organization
+Reference ID
+011103138011</t>
+  </si>
+  <si>
+    <t>100.00
+AED
+Donated to
+Zakat Fund-Zakat Al Mal
+Charity Organization
+Reference ID
+011103138011</t>
+  </si>
+  <si>
+    <t>100.00
+AED
+Donated to
+Zakat Fund-Al Sadaqat
+Charity Organization
+Reference ID
+011103138011</t>
+  </si>
+  <si>
+    <t>100.00
+AED
+Donated to
+Zakat Fund-Zakat Al Fitr
+Charity Organization
+Reference ID
+011103138011</t>
+  </si>
+  <si>
+    <t>50.00
+AED
+Paid To
+FEWA
+FEWA
+210000137777
+Reference ID
+2210348118962</t>
+  </si>
+  <si>
+    <t>50.00
+AED
+(13.66 USD)
+Paid To
+DU
+du Postpaid
+599588538
+Reference ID
+22101848207546</t>
+  </si>
+  <si>
+    <t>200.51
+AED
+Paid To
+ADDC
+ADDC
+8235355929
+Reference ID
+22101151145086</t>
+  </si>
+  <si>
+    <t>50.00
+AED
+Paid To
+SALIK
+SALIK
+32100001
+Reference ID
+2210193752232</t>
+  </si>
+  <si>
+    <t>100.00
+AED
+Transfer to
+Short.name 1074784
+011074784027
+Ajman Bank
+Description
+Reference ID
+FT230964MY46</t>
   </si>
   <si>
     <t>100.00
@@ -336,7 +442,7 @@
 Savings Account
 011103138023
 Reference ID
-FT23093BLCKX</t>
+FT230967R6HX</t>
   </si>
   <si>
     <t>100.00
@@ -347,7 +453,7 @@
 Citibank NA
 Description
 Reference ID
-FT230939R2JC</t>
+FT23096KN0YH</t>
   </si>
   <si>
     <t>2,200.00
@@ -361,7 +467,7 @@
 HDFC BANK LIMITED
 Description
 Reference ID
-FT23093V05WJ</t>
+FT23096RHR1X</t>
   </si>
   <si>
     <t>30.00
@@ -375,7 +481,7 @@
 CHASE INVESTMENT COUNSEL CORPORATION
 Description
 Reference ID
-FT230939W1GG</t>
+FT230960KKMR</t>
   </si>
   <si>
     <t>30.00
@@ -389,7 +495,7 @@
 NATIXIS FACTOR
 Description
 Reference ID
-FT2309370HPQ</t>
+FT230961D78M</t>
   </si>
   <si>
     <t>100.00
@@ -398,28 +504,10 @@
 NASER AL HAT011
 5309 1822 5332 1312
 Reference ID
-FT23093W44DW</t>
-  </si>
-  <si>
-    <t>DonationName</t>
-  </si>
-  <si>
-    <t>Humaid Bin Rashid AL Nouimi</t>
-  </si>
-  <si>
-    <t>Zakat Fund-Zakat Al Mal</t>
-  </si>
-  <si>
-    <t>Zakat Fund-Al Sadaqat</t>
-  </si>
-  <si>
-    <t>Zakat Fund-Zakat Al Fitr</t>
-  </si>
-  <si>
-    <t>Salik</t>
-  </si>
-  <si>
-    <t>SALIK</t>
+FT23096Z3B0T</t>
+  </si>
+  <si>
+    <t>0599588538</t>
   </si>
   <si>
     <t>50.00
@@ -429,7 +517,7 @@
 FEWA
 210000137777
 Reference ID
-2210882987592</t>
+22101469349854</t>
   </si>
   <si>
     <t>50.00
@@ -438,9 +526,9 @@
 Paid To
 DU
 du Postpaid
-599588538
-Reference ID
-22102030850944</t>
+0599588538
+Reference ID
+2210416831275</t>
   </si>
   <si>
     <t>200.51
@@ -450,7 +538,7 @@
 ADDC
 8235355929
 Reference ID
-22101055438748</t>
+22101057041035</t>
   </si>
   <si>
     <t>50.00
@@ -460,48 +548,10 @@
 SALIK
 32100001
 Reference ID
-2210468690840</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-Paid To
-FEWA
-FEWA
-210000137777
-Reference ID
-22101578623579</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-(13.66 USD)
-Paid To
-DU
-du Postpaid
-599588538
-Reference ID
-2210109602264</t>
-  </si>
-  <si>
-    <t>200.51
-AED
-Paid To
-ADDC
-ADDC
-8235355929
-Reference ID
-2210610489252</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-Paid To
-SALIK
-SALIK
-32100001
-Reference ID
-22101983799526</t>
+22101978101086</t>
+  </si>
+  <si>
+    <t>Biller Du Saved Successfully with consumer number 0599588538</t>
   </si>
   <si>
     <t>100.00
@@ -512,7 +562,7 @@
 Ajman Bank
 Description
 Reference ID
-FT23095WW9LF</t>
+FT231034GDQB</t>
   </si>
   <si>
     <t>100.00
@@ -522,7 +572,7 @@
 Savings Account
 011103138023
 Reference ID
-FT23095KJGYM</t>
+FT23103DDP64</t>
   </si>
   <si>
     <t>100.00
@@ -533,7 +583,7 @@
 Citibank NA
 Description
 Reference ID
-FT23095T3JTM</t>
+FT23103Z75ZM</t>
   </si>
   <si>
     <t>2,200.00
@@ -547,7 +597,7 @@
 HDFC BANK LIMITED
 Description
 Reference ID
-FT230956F6VS</t>
+FT231035YWB3</t>
   </si>
   <si>
     <t>30.00
@@ -561,108 +611,7 @@
 CHASE INVESTMENT COUNSEL CORPORATION
 Description
 Reference ID
-FT23095KKHSS</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-Paid To
-FEWA
-FEWA
-210000137777
-Reference ID
-2210569314444</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-(13.66 USD)
-Paid To
-DU
-du Postpaid
-599588538
-Reference ID
-2210976068421</t>
-  </si>
-  <si>
-    <t>200.51
-AED
-Paid To
-ADDC
-ADDC
-8235355929
-Reference ID
-22101905912377</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-Paid To
-SALIK
-SALIK
-32100001
-Reference ID
-22101122318583</t>
-  </si>
-  <si>
-    <t>100.00
-AED
-Transfer to
-Short.name 1074784
-011074784027
-Ajman Bank
-Description
-Reference ID
-FT23095Z5CS4</t>
-  </si>
-  <si>
-    <t>100.00
-USD
-(368.60 AED)
-Transfer to
-Savings Account
-011103138023
-Reference ID
-FT23095F1TCJ</t>
-  </si>
-  <si>
-    <t>100.00
-AED
-Transfer to
-test
-AE400211000000220294021
-Citibank NA
-Description
-Reference ID
-FT23095F5QHQ</t>
-  </si>
-  <si>
-    <t>2,200.00
-INR
-(134.24 AED)
-Submitted
-You will be notified once your payment is successful
-Test
-India
-372073000000786
-HDFC BANK LIMITED
-Description
-Reference ID
-FT23095CL7DQ</t>
-  </si>
-  <si>
-    <t>30.00
-USD
-(142.08 AED)
-Submitted
-You will be notified once your payment is successful
-Terence
-United States Of America
-903013089
-CHASE INVESTMENT COUNSEL CORPORATION
-Description
-Reference ID
-FT23095C086G</t>
+FT231032LWQX</t>
   </si>
   <si>
     <t>30.00
@@ -676,7 +625,7 @@
 NATIXIS FACTOR
 Description
 Reference ID
-FT230950KPPR</t>
+FT23103YQMR0</t>
   </si>
   <si>
     <t>100.00
@@ -685,7 +634,7 @@
 Humaid Bin Rashid AL Nouimi
 Charity Organization
 Reference ID
-011103138011</t>
+FT231036FRRX</t>
   </si>
   <si>
     <t>100.00
@@ -694,7 +643,7 @@
 Zakat Fund-Zakat Al Mal
 Charity Organization
 Reference ID
-011103138011</t>
+FT231036VXWW</t>
   </si>
   <si>
     <t>100.00
@@ -703,7 +652,7 @@
 Zakat Fund-Al Sadaqat
 Charity Organization
 Reference ID
-011103138011</t>
+FT23103JLG6M</t>
   </si>
   <si>
     <t>100.00
@@ -712,78 +661,7 @@
 Zakat Fund-Zakat Al Fitr
 Charity Organization
 Reference ID
-011103138011</t>
-  </si>
-  <si>
-    <t>100.00
-AED
-Paid To
-NASER AL HAT011
-5309 1822 5332 1312
-Reference ID
-FT230950X682</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-Paid To
-FEWA
-FEWA
-210000137777
-Reference ID
-2210348118962</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-(13.66 USD)
-Paid To
-DU
-du Postpaid
-599588538
-Reference ID
-22101848207546</t>
-  </si>
-  <si>
-    <t>200.51
-AED
-Paid To
-ADDC
-ADDC
-8235355929
-Reference ID
-22101151145086</t>
-  </si>
-  <si>
-    <t>50.00
-AED
-Paid To
-SALIK
-SALIK
-32100001
-Reference ID
-2210193752232</t>
-  </si>
-  <si>
-    <t>100.00
-AED
-Transfer to
-Short.name 1074784
-011074784027
-Ajman Bank
-Description
-Reference ID
-FT230964MY46</t>
-  </si>
-  <si>
-    <t>100.00
-USD
-(368.60 AED)
-Transfer to
-Savings Account
-011103138023
-Reference ID
-FT230967R6HX</t>
+FT23103QKNY6</t>
   </si>
   <si>
     <t>100.00
@@ -794,58 +672,7 @@
 Citibank NA
 Description
 Reference ID
-FT23096KN0YH</t>
-  </si>
-  <si>
-    <t>2,200.00
-INR
-(134.24 AED)
-Submitted
-You will be notified once your payment is successful
-Test
-India
-372073000000786
-HDFC BANK LIMITED
-Description
-Reference ID
-FT23096RHR1X</t>
-  </si>
-  <si>
-    <t>30.00
-USD
-(142.08 AED)
-Submitted
-You will be notified once your payment is successful
-Terence
-United States Of America
-903013089
-CHASE INVESTMENT COUNSEL CORPORATION
-Description
-Reference ID
-FT230960KKMR</t>
-  </si>
-  <si>
-    <t>30.00
-USD
-(142.08 AED)
-Submitted
-You will be notified once your payment is successful
-AKS Natixis Bk
-France
-FR7630007999992738468400131
-NATIXIS FACTOR
-Description
-Reference ID
-FT230961D78M</t>
-  </si>
-  <si>
-    <t>100.00
-AED
-Paid To
-NASER AL HAT011
-5309 1822 5332 1312
-Reference ID
-FT23096Z3B0T</t>
+FT23103SGYGB</t>
   </si>
 </sst>
 </file>
@@ -917,7 +744,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -973,6 +800,9 @@
     </xf>
     <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1361,7 +1191,7 @@
         <v>24</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>31</v>
@@ -1381,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>78</v>
@@ -1390,7 +1220,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1398,7 +1228,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>78</v>
@@ -1407,7 +1237,7 @@
         <v>100</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1415,7 +1245,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>78</v>
@@ -1424,7 +1254,7 @@
         <v>100</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1432,7 +1262,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>78</v>
@@ -1441,7 +1271,7 @@
         <v>100</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -1566,7 +1396,7 @@
     <col min="5" max="5" customWidth="true" width="24.42578125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="20.3671875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row ht="15.75" r="1" spans="1:8">
@@ -1613,7 +1443,7 @@
         <v>100</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1633,7 +1463,7 @@
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1646,7 +1476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1683,7 +1513,7 @@
         <v>72</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1759,7 +1589,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1834,7 +1664,7 @@
         <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1847,8 +1677,8 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
-        <v>599588538</v>
+      <c r="D3" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -1863,7 +1693,7 @@
         <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1883,7 +1713,7 @@
         <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1891,10 +1721,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3">
         <v>32100001</v>
@@ -1906,7 +1736,7 @@
         <v>6843</v>
       </c>
       <c r="J5" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1920,7 +1750,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2004,8 +1834,8 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
-        <v>599588538</v>
+      <c r="D3" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -2050,7 +1880,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2134,8 +1964,8 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
-        <v>599588538</v>
+      <c r="D3" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="E3" s="4">
         <v>50</v>
@@ -2148,7 +1978,7 @@
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="7" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2169,7 +1999,7 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2229,7 +2059,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2241,7 +2071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2290,7 +2120,7 @@
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="7" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2350,7 +2180,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2466,7 +2296,7 @@
         <v>2200</v>
       </c>
       <c r="O2" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2504,7 +2334,7 @@
         <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2574,7 +2404,7 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>